<commit_message>
[Change] Unlock Some Sheet Cells
</commit_message>
<xml_diff>
--- a/src/bundlers/resources/template.xlsx
+++ b/src/bundlers/resources/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/douglas/Documents/Projects/Pessoais/Apps/FinanceIB/src/extractors/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/douglas/Documents/Projects/Pessoais/Apps/FinanceIB/src/bundlers/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4086DE-9890-3D49-B935-9089BEFB9DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A237AF9-3C58-144C-AF55-2CE494313D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="640" windowWidth="28040" windowHeight="16940" xr2:uid="{0882606A-3D97-D943-89D1-145F731940E3}"/>
   </bookViews>
@@ -291,7 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -301,7 +301,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -336,9 +335,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -359,6 +355,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -692,61 +692,61 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="30.83203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="30.83203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="8" style="6" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="17.5" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="6"/>
+    <col min="1" max="1" width="12.83203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="30.83203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="8" style="5" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="17.5" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="23"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="24"/>
+      <c r="I3" s="22"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="8">
         <f ca="1">MONTH(TODAY())</f>
         <v>12</v>
       </c>
@@ -755,7 +755,7 @@
       <c r="H5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <f ca="1">YEAR(TODAY())</f>
         <v>2022</v>
       </c>
@@ -764,30 +764,30 @@
       <c r="H6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <f ca="1">TODAY()</f>
-        <v>44925</v>
+        <v>44926</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="6" t="b">
+      <c r="I7" s="5" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="24"/>
+      <c r="I9" s="22"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="7">
         <v>0</v>
       </c>
     </row>
@@ -795,21 +795,21 @@
       <c r="H11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="17"/>
+      <c r="I12" s="23"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H14" s="24" t="s">
+      <c r="H14" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="24"/>
+      <c r="I14" s="22"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H15" s="1" t="s">
@@ -839,7 +839,7 @@
       </c>
     </row>
     <row r="18" spans="8:9" x14ac:dyDescent="0.2">
-      <c r="H18" s="9" t="s">
+      <c r="H18" s="8" t="s">
         <v>16</v>
       </c>
       <c r="I18" s="4">
@@ -848,8 +848,8 @@
       </c>
     </row>
     <row r="19" spans="8:9" x14ac:dyDescent="0.2">
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>

</xml_diff>

<commit_message>
[Feature] Allow Ignore Grouping; Allow Set Custom Output Filename; Get Calculated Data from Spreadsheet
</commit_message>
<xml_diff>
--- a/src/bundlers/resources/template.xlsx
+++ b/src/bundlers/resources/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/douglas/Documents/Projects/Pessoais/Apps/FinanceIB/src/bundlers/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A237AF9-3C58-144C-AF55-2CE494313D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E09CD6-D017-2844-9A8D-D2223790D85D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="640" windowWidth="28040" windowHeight="16940" xr2:uid="{0882606A-3D97-D943-89D1-145F731940E3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Entradas</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Coletados do Extrato</t>
   </si>
   <si>
-    <t>Dados do Relatório (Alterar)</t>
-  </si>
-  <si>
     <t>Disponibilidade</t>
   </si>
   <si>
@@ -93,6 +90,12 @@
   </si>
   <si>
     <t>Quebrar Página?</t>
+  </si>
+  <si>
+    <t>Agrupar Iguais?</t>
+  </si>
+  <si>
+    <t>Configurações do Relatório</t>
   </si>
 </sst>
 </file>
@@ -291,7 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -332,6 +335,10 @@
     <xf numFmtId="14" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -352,13 +359,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -687,7 +687,7 @@
       <pane xSplit="9" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomRight" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -705,16 +705,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="19" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -737,10 +737,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="22"/>
+      <c r="H3" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H4" s="3" t="s">
@@ -748,7 +748,7 @@
       </c>
       <c r="I4" s="8">
         <f ca="1">MONTH(TODAY())</f>
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -757,7 +757,7 @@
       </c>
       <c r="I5" s="5">
         <f ca="1">YEAR(TODAY())</f>
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -766,99 +766,103 @@
       </c>
       <c r="I6" s="6">
         <f ca="1">TODAY()</f>
-        <v>44926</v>
+        <v>44936</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I7" s="5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H9" s="22" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H10" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="22"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="7">
-        <v>0</v>
-      </c>
+      <c r="I10" s="16"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H11" s="3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I11" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H12" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="23"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H14" s="22" t="s">
+      <c r="H12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="15"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H15" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="22"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I16" s="2">
         <f>SUM(B:B)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H16" s="1" t="s">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I17" s="2">
         <f>SUM(E:E)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.2">
-      <c r="H17" s="3" t="s">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I17" s="4">
-        <f>I15-I16</f>
+      <c r="I18" s="4">
+        <f>I16-I17</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.2">
-      <c r="H18" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="4">
-        <f>I10+I17</f>
+    <row r="19" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="4">
+        <f>I11+I18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.2">
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-    </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection sheet="1" selectLockedCells="1"/>
   <mergeCells count="5">
+    <mergeCell ref="H15:I15"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H10:I10"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" error="O mês de apuração deve estar entre 1 (janeiro) e 12 (dezembro)" sqref="I4" xr:uid="{47767305-9961-AC47-A940-5718D6602496}">
@@ -873,7 +877,7 @@
       <formula1>36526</formula1>
       <formula2>73415</formula2>
     </dataValidation>
-    <dataValidation type="list" showErrorMessage="1" error="Insira 1 para &quot;Sim&quot; e 0 para &quot;Não&quot;" sqref="I7" xr:uid="{8CC013BD-DA55-2549-BFD2-45F85C470DEC}">
+    <dataValidation type="list" allowBlank="1" error="Insira 1 para &quot;Sim&quot; e 0 para &quot;Não&quot;" sqref="I7:I8" xr:uid="{8CC013BD-DA55-2549-BFD2-45F85C470DEC}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>